<commit_message>
Update level editor design docs to reflect progress
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C87DB4-D406-47B7-9FED-4A4A1DC0798A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2F8A3-0B4A-4B31-8CC0-65AF2DCBD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -623,7 +623,7 @@
   <dimension ref="B2:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -662,7 +662,7 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F3">
@@ -682,7 +682,7 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
       <c r="F4">
@@ -861,7 +861,7 @@
       </c>
     </row>
     <row r="14" spans="2:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="B14" t="s">
+      <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C14">
@@ -957,7 +957,7 @@
       </c>
     </row>
     <row r="20" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B20" t="s">
+      <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C20">

</xml_diff>

<commit_message>
Create a desired feature list for level editor
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E2F8A3-0B4A-4B31-8CC0-65AF2DCBD7E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE69FF-E220-4258-A3B5-C1600AC3E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
   <si>
     <t>Liked areas of the level editor</t>
   </si>
@@ -234,13 +234,25 @@
   </si>
   <si>
     <t>Cutscenes</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Have objects be customisable</t>
+  </si>
+  <si>
+    <t>Add ability to add custom music to level</t>
+  </si>
+  <si>
+    <t>Add ability to create custom tilesets for levels</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,8 +275,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -274,6 +293,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -295,19 +319,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -623,7 +650,7 @@
   <dimension ref="B2:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -643,7 +670,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
@@ -662,11 +689,11 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>34</v>
+      <c r="E3" t="s">
+        <v>67</v>
       </c>
       <c r="F3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" t="s">
         <v>5</v>
@@ -682,11 +709,11 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>29</v>
+      <c r="E4" t="s">
+        <v>68</v>
       </c>
       <c r="F4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H4" t="s">
         <v>2</v>
@@ -703,7 +730,7 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>69</v>
       </c>
       <c r="F5">
         <v>1</v>
@@ -722,12 +749,6 @@
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
@@ -742,12 +763,6 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
       <c r="H7" t="s">
         <v>4</v>
       </c>
@@ -762,12 +777,6 @@
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
       <c r="H8" t="s">
         <v>3</v>
       </c>
@@ -782,12 +791,6 @@
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
       <c r="H9" t="s">
         <v>1</v>
       </c>
@@ -796,17 +799,11 @@
       </c>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
+      <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C10">
         <v>2</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
       </c>
       <c r="H10" t="s">
         <v>10</v>
@@ -822,12 +819,6 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
       <c r="H11" t="s">
         <v>9</v>
       </c>
@@ -849,29 +840,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>32</v>
       </c>
       <c r="C13">
         <v>2</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="14" spans="2:9" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C14">
         <v>2</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14">
-        <v>8</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>11</v>
@@ -887,12 +869,6 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="E15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
       <c r="H15" t="s">
         <v>17</v>
       </c>
@@ -928,13 +904,19 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
+      <c r="E18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" t="s">
+        <v>7</v>
+      </c>
       <c r="H18" t="s">
         <v>13</v>
       </c>
@@ -942,12 +924,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B19" t="s">
+    <row r="19" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C19">
         <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
       </c>
       <c r="H19" t="s">
         <v>14</v>
@@ -963,6 +951,12 @@
       <c r="C20">
         <v>1</v>
       </c>
+      <c r="E20" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
       <c r="H20" t="s">
         <v>15</v>
       </c>
@@ -977,6 +971,12 @@
       <c r="C21">
         <v>1</v>
       </c>
+      <c r="E21" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
       <c r="H21" t="s">
         <v>16</v>
       </c>
@@ -985,10 +985,16 @@
       </c>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B22" t="s">
+      <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C22">
+        <v>1</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F22">
         <v>1</v>
       </c>
       <c r="H22" t="s">
@@ -1005,6 +1011,12 @@
       <c r="C23">
         <v>1</v>
       </c>
+      <c r="E23" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
       <c r="H23" t="s">
         <v>25</v>
       </c>
@@ -1019,6 +1031,12 @@
       <c r="C24">
         <v>1</v>
       </c>
+      <c r="E24" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
       <c r="H24" t="s">
         <v>45</v>
       </c>
@@ -1033,6 +1051,12 @@
       <c r="C25">
         <v>1</v>
       </c>
+      <c r="E25" t="s">
+        <v>33</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
@@ -1041,11 +1065,23 @@
       <c r="C26">
         <v>1</v>
       </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
       <c r="H26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="27" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E27" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
       <c r="H27" t="s">
         <v>21</v>
       </c>
@@ -1061,7 +1097,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="E29" s="1" t="s">
+        <v>37</v>
+      </c>
       <c r="H29" t="s">
         <v>19</v>
       </c>
@@ -1069,7 +1108,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="E30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
       <c r="H30" t="s">
         <v>24</v>
       </c>
@@ -1078,6 +1123,12 @@
       </c>
     </row>
     <row r="31" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E31" t="s">
+        <v>39</v>
+      </c>
+      <c r="F31">
+        <v>3</v>
+      </c>
       <c r="H31" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Compile feedback from level editor beta
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66AE69FF-E220-4258-A3B5-C1600AC3E824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C2FDFA0-38FF-4498-BEB7-F1A8A7941CD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="80">
   <si>
     <t>Liked areas of the level editor</t>
   </si>
@@ -246,6 +246,36 @@
   </si>
   <si>
     <t>Add ability to create custom tilesets for levels</t>
+  </si>
+  <si>
+    <t>Beta Feedback</t>
+  </si>
+  <si>
+    <t>Add a "Start from Beginning" option with a keyboard shortcut</t>
+  </si>
+  <si>
+    <t>Make a preview sprite for which tile/object you are placing</t>
+  </si>
+  <si>
+    <t>Add a redo button</t>
+  </si>
+  <si>
+    <t>Level editor UI should be more compact</t>
+  </si>
+  <si>
+    <t>Top-left buttons in editor obstruct tile placement</t>
+  </si>
+  <si>
+    <t>Exiting level editor should take you to world menu</t>
+  </si>
+  <si>
+    <t>Eraser button should deselect when selecting a new tile/object</t>
+  </si>
+  <si>
+    <t>Make editable layers (TileMap) visually distinct from non-editable ones (Background)</t>
+  </si>
+  <si>
+    <t>Add Buttons and/or Keyboard Shortcuts to go to the start and end of a level</t>
   </si>
 </sst>
 </file>
@@ -647,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5DDB2B2-9DD4-43B3-A62D-58C786E57E72}">
-  <dimension ref="B2:I36"/>
+  <dimension ref="B2:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -658,11 +688,12 @@
     <col min="1" max="1" width="8.88671875" customWidth="1"/>
     <col min="2" max="2" width="73" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
-    <col min="5" max="5" width="58.88671875" customWidth="1"/>
-    <col min="8" max="8" width="46.21875" customWidth="1"/>
+    <col min="5" max="5" width="74.33203125" customWidth="1"/>
+    <col min="8" max="8" width="59.44140625" customWidth="1"/>
+    <col min="11" max="11" width="45.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="2:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B2" s="1" t="s">
         <v>40</v>
       </c>
@@ -670,19 +701,25 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="I2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="K2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2" t="s">
         <v>56</v>
       </c>
@@ -690,19 +727,25 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3" t="s">
         <v>67</v>
       </c>
-      <c r="F3">
+      <c r="I3">
         <v>3</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="I3">
+      <c r="L3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
         <v>35</v>
       </c>
@@ -710,19 +753,25 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="H4" t="s">
         <v>68</v>
       </c>
-      <c r="F4">
-        <v>2</v>
-      </c>
-      <c r="H4" t="s">
-        <v>2</v>
-      </c>
       <c r="I4">
+        <v>2</v>
+      </c>
+      <c r="K4" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>57</v>
       </c>
@@ -730,117 +779,165 @@
         <v>5</v>
       </c>
       <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="H5" t="s">
         <v>69</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
         <v>6</v>
       </c>
-      <c r="I5">
+      <c r="L5">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
-      <c r="H6" t="s">
+      <c r="E6" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
         <v>8</v>
       </c>
-      <c r="I6">
+      <c r="L6">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>34</v>
       </c>
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="H7" t="s">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
         <v>4</v>
       </c>
-      <c r="I7">
+      <c r="L7">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>41</v>
       </c>
       <c r="C8">
         <v>3</v>
       </c>
-      <c r="H8" t="s">
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="K8" t="s">
         <v>3</v>
       </c>
-      <c r="I8">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C9">
         <v>2</v>
       </c>
-      <c r="H9" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+      <c r="L9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
         <v>50</v>
       </c>
       <c r="C10">
         <v>2</v>
       </c>
-      <c r="H10" t="s">
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
         <v>10</v>
       </c>
-      <c r="I10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="H11" t="s">
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
         <v>9</v>
       </c>
-      <c r="I11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>31</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="H12" t="s">
+      <c r="E12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="K12" t="s">
         <v>26</v>
       </c>
-      <c r="I12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>32</v>
       </c>
@@ -848,326 +945,326 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="2:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
         <v>61</v>
       </c>
       <c r="C14">
         <v>2</v>
       </c>
-      <c r="H14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="I14" t="s">
+      <c r="L14" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="15" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>60</v>
       </c>
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="H15" t="s">
+      <c r="K15" t="s">
         <v>17</v>
       </c>
-      <c r="I15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>47</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
-      <c r="H16" t="s">
+      <c r="K16" t="s">
         <v>12</v>
       </c>
-      <c r="I16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>44</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
-      <c r="H17" t="s">
+      <c r="K17" t="s">
         <v>18</v>
       </c>
-      <c r="I17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="L17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>51</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F18" t="s">
+      <c r="I18" t="s">
         <v>7</v>
       </c>
-      <c r="H18" t="s">
+      <c r="K18" t="s">
         <v>13</v>
       </c>
-      <c r="I18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="L18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B19" s="3" t="s">
         <v>46</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="H19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F19">
-        <v>2</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19">
+        <v>2</v>
+      </c>
+      <c r="K19" t="s">
         <v>14</v>
       </c>
-      <c r="I19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>48</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="H20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="H20" t="s">
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
         <v>15</v>
       </c>
-      <c r="I20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>52</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="H21" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="H21" t="s">
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
         <v>16</v>
       </c>
-      <c r="I21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B22" s="3" t="s">
         <v>53</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="H22" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="H22" t="s">
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
         <v>27</v>
       </c>
-      <c r="I22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>54</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
-      <c r="E23" t="s">
+      <c r="H23" t="s">
         <v>31</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
         <v>25</v>
       </c>
-      <c r="I23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>55</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
-      <c r="E24" t="s">
+      <c r="H24" t="s">
         <v>32</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
         <v>45</v>
       </c>
-      <c r="I24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="L24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>58</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
-      <c r="E25" t="s">
+      <c r="H25" t="s">
         <v>33</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="I25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
       <c r="B26" t="s">
         <v>59</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="H26" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="H26" s="1" t="s">
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="K26" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E27" s="2" t="s">
+    <row r="27" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H27" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="K27" t="s">
         <v>21</v>
       </c>
-      <c r="I27">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="H28" t="s">
+      <c r="L27">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="K28" t="s">
         <v>23</v>
       </c>
-      <c r="I28">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="29" spans="2:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="E29" s="1" t="s">
+      <c r="L28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="H29" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H29" t="s">
+      <c r="K29" t="s">
         <v>19</v>
       </c>
-      <c r="I29">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="30" spans="2:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="E30" s="2" t="s">
+      <c r="L29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="H30" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="F30">
+      <c r="I30">
         <v>8</v>
       </c>
-      <c r="H30" t="s">
+      <c r="K30" t="s">
         <v>24</v>
       </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="E31" t="s">
+      <c r="L30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
         <v>39</v>
       </c>
-      <c r="F31">
+      <c r="I31">
         <v>3</v>
       </c>
-      <c r="H31" t="s">
+      <c r="K31" t="s">
         <v>22</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="8:9" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H33" s="1" t="s">
+      <c r="L31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="11:12" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="K33" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="34" spans="8:9" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="H34" t="s">
+    <row r="34" spans="11:12" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="K34" t="s">
         <v>63</v>
       </c>
-      <c r="I34">
+      <c r="L34">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H35" t="s">
+    <row r="35" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K35" t="s">
         <v>64</v>
       </c>
-      <c r="I35">
+      <c r="L35">
         <v>9</v>
       </c>
     </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.3">
-      <c r="H36" t="s">
+    <row r="36" spans="11:12" x14ac:dyDescent="0.3">
+      <c r="K36" t="s">
         <v>65</v>
       </c>
-      <c r="I36">
+      <c r="L36">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H3:I12">
-    <sortCondition descending="1" ref="I3:I12"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="K3:L12">
+    <sortCondition descending="1" ref="L3:L12"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Editor: Preview icon for the tile/object you're about to place
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E79942-6404-4C55-BF39-39289240C62B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A6117D-6AAF-4976-8D35-713EF41E4B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <dimension ref="B2:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -729,10 +729,10 @@
       <c r="C3">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>1</v>
       </c>
       <c r="H3" t="s">
@@ -755,10 +755,10 @@
       <c r="C4">
         <v>6</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>1</v>
       </c>
       <c r="H4" t="s">

</xml_diff>

<commit_message>
Editor Play from Start button
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9A6117D-6AAF-4976-8D35-713EF41E4B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03145ECB-4DFC-453A-A210-9A05D36BDAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <dimension ref="B2:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="E5" sqref="E5:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -781,10 +781,10 @@
       <c r="C5">
         <v>5</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>1</v>
       </c>
       <c r="H5" t="s">

</xml_diff>

<commit_message>
ObjectMaps are no longer placeable in worldmaps
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03145ECB-4DFC-453A-A210-9A05D36BDAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC67EDA-6A45-49C3-B012-28F745783247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -683,7 +683,7 @@
   <dimension ref="B2:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5:F5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -827,10 +827,10 @@
       <c r="C7">
         <v>3</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>1</v>
       </c>
       <c r="K7" t="s">
@@ -907,12 +907,6 @@
       <c r="C11">
         <v>2</v>
       </c>
-      <c r="E11" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
       <c r="K11" t="s">
         <v>9</v>
       </c>
@@ -928,7 +922,7 @@
         <v>2</v>
       </c>
       <c r="E12" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -948,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="E13" t="s">
-        <v>80</v>
+        <v>68</v>
       </c>
       <c r="F13">
         <v>1</v>
@@ -974,6 +968,12 @@
       </c>
       <c r="C15">
         <v>2</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
       </c>
       <c r="K15" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
Fix levels appearing in the wrong order in Open Level menu
</commit_message>
<xml_diff>
--- a/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
+++ b/Documentation/Level Editor/Feedback Survey/Level Editor Feedback Compiled.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alex\SuperTux-Classic\Documentation\Level Editor\Feedback Survey\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBC67EDA-6A45-49C3-B012-28F745783247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C11E25-9870-4A30-AD8C-1DC00F1DF847}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C9BF8C9A-5AA6-4F7F-ADE8-FF66396A48DF}"/>
   </bookViews>
@@ -921,10 +921,10 @@
       <c r="C12">
         <v>2</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>1</v>
       </c>
       <c r="K12" t="s">

</xml_diff>